<commit_message>
final as per requirements
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aviis\OneDrive\Documents\Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aviis\OneDrive\Documents\GitHub\WhoseNext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A11231-6D9F-4D53-95CD-7E88D317118F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530AA53F-C8AD-4CA8-B192-939CDEBCFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C8B4E50-EEB5-4286-AFD3-D472239B34ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Room</t>
+  </si>
+  <si>
+    <t>Shrikt</t>
+  </si>
+  <si>
+    <t>405,HR,Hall</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AED251-BAA5-4C54-BE86-926C2F69EA36}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,6 +443,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added excel write feature
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aviis\OneDrive\Documents\GitHub\WhoseNext\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b2a918fad6f5764/Documents/GitHub/WhoseNext/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530AA53F-C8AD-4CA8-B192-939CDEBCFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{530AA53F-C8AD-4CA8-B192-939CDEBCFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F05FF7D6-F586-4D23-B2BF-DDC3CB205EB1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C8B4E50-EEB5-4286-AFD3-D472239B34ED}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>302b,405c</t>
   </si>
   <si>
-    <t>Aajarsh</t>
-  </si>
-  <si>
     <t>Room</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>405,HR,Hall</t>
+  </si>
+  <si>
+    <t>Aakarsh</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +424,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -437,7 +437,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -445,10 +445,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor change in interview card appearence
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b2a918fad6f5764/Documents/GitHub/WhoseNext/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{530AA53F-C8AD-4CA8-B192-939CDEBCFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F05FF7D6-F586-4D23-B2BF-DDC3CB205EB1}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{530AA53F-C8AD-4CA8-B192-939CDEBCFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8C5AE4-B3FA-49FC-8362-4E089E60EAD3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C8B4E50-EEB5-4286-AFD3-D472239B34ED}"/>
   </bookViews>
@@ -39,22 +39,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Avikshit</t>
-  </si>
-  <si>
-    <t>302b,405c</t>
-  </si>
-  <si>
     <t>Room</t>
   </si>
   <si>
-    <t>Shrikt</t>
-  </si>
-  <si>
-    <t>405,HR,Hall</t>
-  </si>
-  <si>
-    <t>Aakarsh</t>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>302,403,506</t>
+  </si>
+  <si>
+    <t>506,102</t>
   </si>
 </sst>
 </file>
@@ -90,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,6 +109,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,13 +415,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -424,31 +429,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>302</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>